<commit_message>
reset filter is added, Thermistor removed and the testpoint connections to the JP1 are removed
</commit_message>
<xml_diff>
--- a/LBM313/BOM_NBMC_LBM313.xlsx
+++ b/LBM313/BOM_NBMC_LBM313.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="47" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="82" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Partlist" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="225">
   <si>
     <r>
       <t xml:space="preserve">NBMC health Monitor Part List  </t>
@@ -34,7 +34,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(11/26/2014)</t>
+      <t xml:space="preserve">(12/1/2014)</t>
     </r>
   </si>
   <si>
@@ -135,7 +135,7 @@
     <t>GRM155R71H152KA01D</t>
   </si>
   <si>
-    <t>C20</t>
+    <t>C20,C32</t>
   </si>
   <si>
     <t>1nF capacitor</t>
@@ -177,18 +177,30 @@
     <t>C3</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>100uF capacitor</t>
   </si>
   <si>
-    <t>C_100uF_0402</t>
+    <t>C_100uF_1210</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>TAJB107M006RNJ</t>
+  </si>
+  <si>
+    <t>581-TAJB107M006R</t>
+  </si>
+  <si>
+    <t>Capacitor, 100uF, 0402, 20%, 6.3V</t>
   </si>
   <si>
     <t>G2</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>Battery Holder</t>
   </si>
   <si>
@@ -198,7 +210,18 @@
     <t>BH2040</t>
   </si>
   <si>
-    <t>Attached with double sided tape, pins soldered to flex tab </t>
+    <r>
+      <t xml:space="preserve">Already purchased – </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Attached with double sided tape, pins soldered to flex tab</t>
+    </r>
   </si>
   <si>
     <t>JP1</t>
@@ -228,17 +251,16 @@
     <t>4 pin connector</t>
   </si>
   <si>
-    <t>To Connect to Berkley Sensor. (Not to be purchased)</t>
+    <t>Not to be purchased - Connect to Berkley Sensor</t>
   </si>
   <si>
     <t>MOD1</t>
   </si>
   <si>
-    <t>(16x12mm)
-LGA</t>
-  </si>
-  <si>
-    <t>Bluetooth Low Energy Module with Integrated Antenna and Balun Chip</t>
+    <t>16mm X 12mm</t>
+  </si>
+  <si>
+    <t>BLE Module with Antenna</t>
   </si>
   <si>
     <t>LBM313-2540</t>
@@ -270,9 +292,6 @@
     <t>ECS-.327-12.5-12-TR</t>
   </si>
   <si>
-    <t>520-.327-12.5-12-TR</t>
-  </si>
-  <si>
     <t>Crystal, 32.768 kHz, 12.5pF, 20/50 ppm,SMD package</t>
   </si>
   <si>
@@ -303,7 +322,19 @@
     <t>RC0402FR-071ML</t>
   </si>
   <si>
-    <t>R15,R16,R17,R18,R26,R27,R181,R182</t>
+    <t>R181,R182</t>
+  </si>
+  <si>
+    <t>330Kohm resistor</t>
+  </si>
+  <si>
+    <t>R_330K_0402_F</t>
+  </si>
+  <si>
+    <t>RC0402FR-07330KL</t>
+  </si>
+  <si>
+    <t>R15,R16,R17,R18,R26,R27</t>
   </si>
   <si>
     <t>10Mohm resistor</t>
@@ -342,12 +373,36 @@
     <t>R191</t>
   </si>
   <si>
+    <t>50Kohm resistor</t>
+  </si>
+  <si>
     <t>Themistor – Resistor</t>
   </si>
   <si>
+    <t>CRCW040250K0FKED</t>
+  </si>
+  <si>
+    <t>71-CRCW040250K0FKED</t>
+  </si>
+  <si>
     <t>High Tolerance Resistor</t>
   </si>
   <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>4.7Kohm resistor</t>
+  </si>
+  <si>
+    <t>R_4.7K_0402_F</t>
+  </si>
+  <si>
+    <t>SG73P1ETTP4701F</t>
+  </si>
+  <si>
+    <t>Filter Component</t>
+  </si>
+  <si>
     <t>R20</t>
   </si>
   <si>
@@ -379,9 +434,6 @@
   </si>
   <si>
     <t>658-CR2032</t>
-  </si>
-  <si>
-    <t>Contained in battery holder</t>
   </si>
   <si>
     <t>U3</t>
@@ -409,9 +461,6 @@
     <t>TP1-8</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Test Points</t>
   </si>
   <si>
@@ -430,6 +479,9 @@
     <t>Themistor</t>
   </si>
   <si>
+    <t>TBD</t>
+  </si>
+  <si>
     <t>Berkley printed sensor; one thermister on bottom side</t>
   </si>
   <si>
@@ -439,7 +491,7 @@
     <t>Berkley printed sensor two gold electrodes on bottom side</t>
   </si>
   <si>
-    <t>Total : </t>
+    <t>Total :</t>
   </si>
   <si>
     <t>ECG Sensor and Battery Extra from nelist</t>
@@ -494,6 +546,9 @@
   </si>
   <si>
     <t>1.5nF</t>
+  </si>
+  <si>
+    <t>C20</t>
   </si>
   <si>
     <t>1nF</t>
@@ -680,7 +735,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -755,6 +810,34 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF00CC33"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF330000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF3300"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFFF3333"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -834,7 +917,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -931,83 +1014,115 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1025,10 +1140,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1044,13 +1155,13 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00CC00"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -1059,7 +1170,7 @@
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
@@ -1087,13 +1198,13 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FFFF3300"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00CC33"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF330000"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
@@ -1114,7 +1225,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="85" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1147,7 +1258,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1301,7 +1412,7 @@
         <f aca="false">CONCATENATE("81-",G6)</f>
         <v>81-GRM155R71C104KA88D</v>
       </c>
-      <c r="J6" s="18"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
@@ -1334,7 +1445,7 @@
       </c>
       <c r="J7" s="18"/>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
         <v>33</v>
       </c>
@@ -1348,7 +1459,7 @@
         <v>35</v>
       </c>
       <c r="E8" s="19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>14</v>
@@ -1433,560 +1544,625 @@
       <c r="A11" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="14" t="n">
+        <v>1210</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="D11" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="E11" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="27"/>
+      <c r="G11" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
-        <v>50</v>
+      <c r="A12" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="15" t="n">
         <v>1</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
-      <c r="J12" s="14" t="s">
-        <v>54</v>
+      <c r="J12" s="28" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="40.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="15" t="n">
         <v>1</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="31" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>63</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="25" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="29"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="29"/>
+      <c r="J14" s="33" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E15" s="19" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="25.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="32" t="s">
-        <v>70</v>
+      <c r="A16" s="34" t="s">
+        <v>74</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E16" s="15" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="30" t="s">
-        <v>76</v>
+      <c r="I16" s="17" t="str">
+        <f aca="false">CONCATENATE("520-",G16)</f>
+        <v>520-ECS-.327-12.5-12-TR</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B17" s="18" t="n">
         <v>402</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E17" s="19" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H17" s="17" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="17" t="str">
-        <f aca="false">CONCATENATE("603-",G25)</f>
-        <v>603-CR2032</v>
+        <f aca="false">CONCATENATE("603-",G17)</f>
+        <v>603-RC0402FR-07100KL</v>
       </c>
       <c r="J17" s="17"/>
     </row>
-    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B18" s="18" t="n">
         <v>402</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E18" s="19" t="n">
         <v>2</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H18" s="17" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="17" t="str">
-        <f aca="false">CONCATENATE("603-",G12)</f>
-        <v>603-BH2040</v>
+        <f aca="false">CONCATENATE("603-",G18)</f>
+        <v>603-RC0402FR-071ML</v>
       </c>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="18" t="n">
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="36" t="n">
         <v>402</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="19" t="n">
-        <v>8</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" s="17" t="s">
+      <c r="C19" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="D19" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="J19" s="18"/>
-    </row>
-    <row r="20" s="33" customFormat="true" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I19" s="35" t="str">
+        <f aca="false">CONCATENATE("603-",G19)</f>
+        <v>603-RC0402FR-07330KL</v>
+      </c>
+      <c r="J19" s="36"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B20" s="18" t="n">
         <v>402</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E20" s="19" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J20" s="18"/>
     </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" s="14" t="n">
+    <row r="21" s="39" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="18" t="n">
         <v>402</v>
       </c>
-      <c r="C21" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="J21" s="16" t="s">
+      <c r="C21" s="17" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="22" s="36" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17" t="s">
+      <c r="D21" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="18" t="n">
+      <c r="E21" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="41" t="n">
         <v>402</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" s="41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="41" t="n">
+        <v>402</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="35" t="str">
+        <f aca="false">CONCATENATE("660-",G23)</f>
+        <v>660-SG73P1ETTP4701F</v>
+      </c>
+      <c r="J23" s="41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="18" t="n">
+        <v>402</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" s="17" t="s">
+      <c r="G24" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="17" t="str">
-        <f aca="false">CONCATENATE("603-",G19)</f>
-        <v>603-RK73H1ETTP1005F</v>
-      </c>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="18" t="n">
+      <c r="I24" s="17" t="str">
+        <f aca="false">CONCATENATE("603-",G24)</f>
+        <v>603-RC0402FR-071ML</v>
+      </c>
+      <c r="J24" s="18"/>
+    </row>
+    <row r="25" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="18" t="n">
         <v>402</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="19" t="n">
+      <c r="C25" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="F23" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H23" s="17" t="s">
+      <c r="F25" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H25" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="17" t="e">
-        <f aca="false">CONCATENATE("603-",G16)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="18"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="E25" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="H25" s="13" t="s">
+      <c r="I25" s="17" t="str">
+        <f aca="false">CONCATENATE("603-",G25)</f>
+        <v>603-RC0402FR-07180KL</v>
+      </c>
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="H26" s="17" t="s">
+      <c r="I27" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="H28" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="J26" s="18"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" s="37" t="n">
+      <c r="I28" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="45" t="n">
         <v>8</v>
       </c>
-      <c r="F27" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="G27" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="I27" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="J27" s="25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" s="36" customFormat="true" ht="18.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" s="40" t="n">
-        <v>1</v>
-      </c>
-      <c r="F28" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="I28" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="J28" s="41" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43" t="n">
-        <v>1</v>
-      </c>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="41" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="44"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
+      <c r="F29" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="J29" s="33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" s="44" customFormat="true" ht="18.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="47"/>
       <c r="D30" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="E30" s="47" t="n">
-        <f aca="false">SUM(E3:E29)</f>
-        <v>47</v>
-      </c>
-      <c r="F30" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="45"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>141</v>
+      </c>
+      <c r="E30" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="H30" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="I30" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="J30" s="49" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="47"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="49" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="52"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" s="55" t="n">
+        <f aca="false">SUM(E3:E31)</f>
+        <v>51</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="53"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1997,13 +2173,10 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="F32:I32"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="J12" r:id="rId1" display="Attached with double sided tape, pins soldered to flex tab"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2033,39 +2206,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AO3" s="0" t="n">
         <v>1</v>
@@ -2073,19 +2246,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="Y4" s="0" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="AF4" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AO4" s="0" t="n">
         <v>1</v>
@@ -2096,16 +2269,16 @@
         <v>21</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="AE5" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AN5" s="0" t="n">
         <v>1</v>
@@ -2113,19 +2286,19 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="AD6" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AM6" s="0" t="n">
         <v>1</v>
@@ -2133,19 +2306,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="W7" s="0" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="AD7" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AM7" s="0" t="n">
         <v>1</v>
@@ -2156,16 +2329,16 @@
         <v>29</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="AD8" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AM8" s="0" t="n">
         <v>1</v>
@@ -2173,19 +2346,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="AF9" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AO9" s="0" t="n">
         <v>1</v>
@@ -2196,16 +2369,16 @@
         <v>37</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="V10" s="0" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="AC10" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AL10" s="0" t="n">
         <v>1</v>
@@ -2213,19 +2386,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="P11" s="0" t="n">
         <v>1</v>
@@ -2233,19 +2406,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="X12" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AE12" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AN12" s="0" t="n">
         <v>1</v>
@@ -2253,19 +2426,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AC13" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AL13" s="0" t="n">
         <v>1</v>
@@ -2273,19 +2446,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="X14" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE14" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="S14" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="X14" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="AE14" s="0" t="s">
-        <v>144</v>
       </c>
       <c r="AN14" s="0" t="n">
         <v>1</v>
@@ -2293,19 +2466,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="W15" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AD15" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AM15" s="0" t="n">
         <v>1</v>
@@ -2313,19 +2486,19 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="W16" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AD16" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AM16" s="0" t="n">
         <v>1</v>
@@ -2333,19 +2506,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AD17" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AM17" s="0" t="n">
         <v>1</v>
@@ -2353,19 +2526,19 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="R18" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="W18" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AD18" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AM18" s="0" t="n">
         <v>1</v>
@@ -2373,19 +2546,19 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="V19" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AC19" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AL19" s="0" t="n">
         <v>1</v>
@@ -2393,19 +2566,19 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="X20" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AE20" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AN20" s="0" t="n">
         <v>1</v>
@@ -2413,19 +2586,19 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="S21" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="X21" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AE21" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AN21" s="0" t="n">
         <v>1</v>
@@ -2433,19 +2606,19 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="Q22" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="V22" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AC22" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AL22" s="0" t="n">
         <v>1</v>
@@ -2453,19 +2626,19 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="Q23" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="V23" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AC23" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AL23" s="0" t="n">
         <v>1</v>
@@ -2473,19 +2646,19 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>154</v>
-      </c>
       <c r="R24" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="W24" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AD24" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AM24" s="0" t="n">
         <v>1</v>
@@ -2493,19 +2666,19 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="R25" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="F25" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="R25" s="0" t="s">
-        <v>155</v>
-      </c>
       <c r="W25" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AD25" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AM25" s="0" t="n">
         <v>1</v>
@@ -2513,19 +2686,19 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q26" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="V26" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="F26" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q26" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="V26" s="0" t="s">
-        <v>156</v>
-      </c>
       <c r="AC26" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AL26" s="0" t="n">
         <v>1</v>
@@ -2533,19 +2706,19 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="Q27" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="V27" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AC27" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AL27" s="0" t="n">
         <v>1</v>
@@ -2553,19 +2726,19 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="V28" s="0" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="AC28" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="AL28" s="0" t="n">
         <v>1</v>
@@ -2573,19 +2746,19 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="S29" s="0" t="n">
         <v>1</v>
@@ -2593,19 +2766,19 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="V30" s="0" t="n">
         <v>1</v>
@@ -2641,157 +2814,157 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>